<commit_message>
fixed minor formatting bugs
</commit_message>
<xml_diff>
--- a/data/excel/actus-tests-future.xlsx
+++ b/data/excel/actus-tests-future.xlsx
@@ -122,7 +122,7 @@
     <t>2020-03-30T00:00:00</t>
   </si>
   <si>
-    <t>0D</t>
+    <t>P0D</t>
   </si>
   <si>
     <t>S</t>
@@ -155,7 +155,7 @@
     <t>future05</t>
   </si>
   <si>
-    <t>3D</t>
+    <t>P3D</t>
   </si>
   <si>
     <t>future06</t>
@@ -194,7 +194,7 @@
     <t>future13</t>
   </si>
   <si>
-    <t>5D</t>
+    <t>P5D</t>
   </si>
   <si>
     <t>future14</t>
@@ -237,7 +237,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -278,6 +278,10 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="10.0"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -311,7 +315,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -356,6 +360,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -41332,48 +41342,48 @@
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="15">
         <v>0.0</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="16">
         <v>0.0</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="7">
+      <c r="G4" s="15">
         <v>-39.67</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="15">
         <v>-39.67</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="16">
         <v>0.0</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="15">
         <v>-39.67</v>
       </c>
     </row>
@@ -41491,7 +41501,7 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="15" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="7" t="s">
@@ -41506,7 +41516,7 @@
       <c r="E2" s="8">
         <v>0.0</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="15" t="s">
         <v>56</v>
       </c>
       <c r="G2" s="7">
@@ -41601,48 +41611,48 @@
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="7" t="s">
+      <c r="A4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="15">
         <v>0.0</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="16">
         <v>0.0</v>
       </c>
-      <c r="F4" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="7">
+      <c r="F4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="15">
         <v>-16.3</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="15">
         <v>-16.3</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="16">
         <v>0.0</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="7">
+      <c r="F5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="15">
         <v>-16.3</v>
       </c>
     </row>

</xml_diff>